<commit_message>
Update README.md and events data
</commit_message>
<xml_diff>
--- a/src/output/events_mumbai_20260203.xlsx
+++ b/src/output/events_mumbai_20260203.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:J31"/>
+  <dimension ref="A1:J61"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,12 +488,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Daily Ka Kaam Hai By Aakash Gupta Mumbai</t>
+          <t>Sama A Festival Of Sufi Music</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>Daily Ka Kaam Hai By Aakash Gupta - MumbaiSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 599 onwardsDaily Ka Kaam Hai By Aakash Gupta - MumbaiLove, Death &amp; Ketchup by Varun GroverBal Gandharva Rang Mandir: MumbaiStand up Comedy₹ 799 onwardsLove, Death &amp; Ketchup by Varun GroverKeinemusik - Live in MumbaiMahalaxmi Race Course: MumbaiConcerts₹ 3500 onwardsKeinemusik - Live in MumbaiSama'a: Festival of Sufi Music - Day 2Tata Theatre: NCPAConcerts₹ 300 onwardsSama'a: Festival of Sufi Music - Day 2</t>
+          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -513,7 +513,7 @@
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/daily-ka-kaam-hai-by-aakash-gupta-mumbai/ET00429299</t>
+          <t>https://in.bookmyshow.com/events/sama-a-festival-of-sufi-music/ET00480911?webview=true</t>
         </is>
       </c>
       <c r="G2" t="inlineStr">
@@ -528,24 +528,24 @@
       </c>
       <c r="I2" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:43</t>
+          <t>2026-02-03 19:33:54</t>
         </is>
       </c>
       <c r="J2" t="inlineStr">
         <is>
-          <t>8801684389609160</t>
+          <t>8514438716691050</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Love Death Ketchup By Varun Grover</t>
+          <t>The Dj Blues 2 And 1 Salsa Elementary Workshop</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Daily Ka Kaam Hai By Aakash Gupta - MumbaiSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 599 onwardsDaily Ka Kaam Hai By Aakash Gupta - MumbaiLove, Death &amp; Ketchup by Varun GroverBal Gandharva Rang Mandir: MumbaiStand up Comedy₹ 799 onwardsLove, Death &amp; Ketchup by Varun GroverKeinemusik - Live in MumbaiMahalaxmi Race Course: MumbaiConcerts₹ 3500 onwardsKeinemusik - Live in MumbaiSama'a: Festival of Sufi Music - Day 2Tata Theatre: NCPAConcerts₹ 300 onwardsSama'a: Festival of Sufi Music - Day 2</t>
+          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -565,7 +565,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/love-death-ketchup-by-varun-grover/ET00466188</t>
+          <t>https://in.bookmyshow.com/events/the-dj-blues-2-and-1-salsa-elementary-workshop/ET00482759?webview=true</t>
         </is>
       </c>
       <c r="G3" t="inlineStr">
@@ -580,24 +580,24 @@
       </c>
       <c r="I3" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:43</t>
+          <t>2026-02-03 19:33:53</t>
         </is>
       </c>
       <c r="J3" t="inlineStr">
         <is>
-          <t>-599795242289484</t>
+          <t>1796954576447607</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Keinemusik Live In Mumbai</t>
+          <t>The Soi Spring 2026 Season</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>Daily Ka Kaam Hai By Aakash Gupta - MumbaiSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 599 onwardsDaily Ka Kaam Hai By Aakash Gupta - MumbaiLove, Death &amp; Ketchup by Varun GroverBal Gandharva Rang Mandir: MumbaiStand up Comedy₹ 799 onwardsLove, Death &amp; Ketchup by Varun GroverKeinemusik - Live in MumbaiMahalaxmi Race Course: MumbaiConcerts₹ 3500 onwardsKeinemusik - Live in MumbaiSama'a: Festival of Sufi Music - Day 2Tata Theatre: NCPAConcerts₹ 300 onwardsSama'a: Festival of Sufi Music - Day 2</t>
+          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -617,7 +617,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/keinemusik-live-in-mumbai/ET00467697</t>
+          <t>https://in.bookmyshow.com/events/the-soi-spring-2026-season/ET00473378?webview=true</t>
         </is>
       </c>
       <c r="G4" t="inlineStr">
@@ -632,24 +632,24 @@
       </c>
       <c r="I4" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:43</t>
+          <t>2026-02-03 19:33:53</t>
         </is>
       </c>
       <c r="J4" t="inlineStr">
         <is>
-          <t>-119528849040579</t>
+          <t>5897986854312311</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>Sama A Festival Of Sufi Music Day 2</t>
+          <t>Vocal Workshop</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Daily Ka Kaam Hai By Aakash Gupta - MumbaiSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 599 onwardsDaily Ka Kaam Hai By Aakash Gupta - MumbaiLove, Death &amp; Ketchup by Varun GroverBal Gandharva Rang Mandir: MumbaiStand up Comedy₹ 799 onwardsLove, Death &amp; Ketchup by Varun GroverKeinemusik - Live in MumbaiMahalaxmi Race Course: MumbaiConcerts₹ 3500 onwardsKeinemusik - Live in MumbaiSama'a: Festival of Sufi Music - Day 2Tata Theatre: NCPAConcerts₹ 300 onwardsSama'a: Festival of Sufi Music - Day 2</t>
+          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -669,7 +669,7 @@
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/sama-a-festival-of-sufi-music-day-2/ET00480908</t>
+          <t>https://in.bookmyshow.com/events/vocal-workshop/ET00393019?webview=true</t>
         </is>
       </c>
       <c r="G5" t="inlineStr">
@@ -684,24 +684,24 @@
       </c>
       <c r="I5" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:43</t>
+          <t>2026-02-03 19:33:53</t>
         </is>
       </c>
       <c r="J5" t="inlineStr">
         <is>
-          <t>-321794354107730</t>
+          <t>8896685463034552</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>Anuv Jain Dastakhat India Tour Mumbai</t>
+          <t>Pookie Jams The Premium Jamming Experience</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>Anuv Jain - Dastakhat India Tour (Mumbai)DOME, SVP Stadium: MumbaiConcerts₹ 2500 onwardsAnuv Jain - Dastakhat India Tour (Mumbai)CALVIN HARRIS - Live in MumbaiInfinity Bay: MumbaiConcerts₹ 3000 onwardsCALVIN HARRIS - Live in MumbaiBhajan Clubbing - The New Wave of DevotionRangasharda Auditorium: MumbaiConcerts₹ 299 onwardsBhajan Clubbing - The New Wave of DevotionGaurav Gupta Live - India TourFine Arts Society (Sivaswamy Auditorium): ChemburStand up Comedy₹ 799 onwardsGaurav Gupta Live - India Tour</t>
+          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -721,7 +721,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/anuv-jain-dastakhat-india-tour-mumbai/ET00470487</t>
+          <t>https://in.bookmyshow.com/events/pookie-jams-the-premium-jamming-experience/ET00461172?webview=true</t>
         </is>
       </c>
       <c r="G6" t="inlineStr">
@@ -736,24 +736,24 @@
       </c>
       <c r="I6" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:44</t>
+          <t>2026-02-03 19:33:52</t>
         </is>
       </c>
       <c r="J6" t="inlineStr">
         <is>
-          <t>6193409027485856</t>
+          <t>-876967374281815</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>Calvin Harris Live In Mumbai</t>
+          <t>Laptop Dj Workshop</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>Anuv Jain - Dastakhat India Tour (Mumbai)DOME, SVP Stadium: MumbaiConcerts₹ 2500 onwardsAnuv Jain - Dastakhat India Tour (Mumbai)CALVIN HARRIS - Live in MumbaiInfinity Bay: MumbaiConcerts₹ 3000 onwardsCALVIN HARRIS - Live in MumbaiBhajan Clubbing - The New Wave of DevotionRangasharda Auditorium: MumbaiConcerts₹ 299 onwardsBhajan Clubbing - The New Wave of DevotionGaurav Gupta Live - India TourFine Arts Society (Sivaswamy Auditorium): ChemburStand up Comedy₹ 799 onwardsGaurav Gupta Live - India Tour</t>
+          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -773,7 +773,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/calvin-harris-live-in-mumbai/ET00462236</t>
+          <t>https://in.bookmyshow.com/events/laptop-dj-workshop/ET00425192?webview=true</t>
         </is>
       </c>
       <c r="G7" t="inlineStr">
@@ -788,24 +788,24 @@
       </c>
       <c r="I7" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:44</t>
+          <t>2026-02-03 19:33:52</t>
         </is>
       </c>
       <c r="J7" t="inlineStr">
         <is>
-          <t>6301505570597666</t>
+          <t>4737487912185766</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>Bhajan Clubbing The New Wave Of Devotion</t>
+          <t>Sunburn Upcoming Events</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>Anuv Jain - Dastakhat India Tour (Mumbai)DOME, SVP Stadium: MumbaiConcerts₹ 2500 onwardsAnuv Jain - Dastakhat India Tour (Mumbai)CALVIN HARRIS - Live in MumbaiInfinity Bay: MumbaiConcerts₹ 3000 onwardsCALVIN HARRIS - Live in MumbaiBhajan Clubbing - The New Wave of DevotionRangasharda Auditorium: MumbaiConcerts₹ 299 onwardsBhajan Clubbing - The New Wave of DevotionGaurav Gupta Live - India TourFine Arts Society (Sivaswamy Auditorium): ChemburStand up Comedy₹ 799 onwardsGaurav Gupta Live - India Tour</t>
+          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -825,7 +825,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/bhajan-clubbing-the-new-wave-of-devotion/ET00481773</t>
+          <t>https://in.bookmyshow.com/events/sunburn-upcoming-events/ET00463644?webview=true</t>
         </is>
       </c>
       <c r="G8" t="inlineStr">
@@ -840,24 +840,24 @@
       </c>
       <c r="I8" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:44</t>
+          <t>2026-02-03 19:33:52</t>
         </is>
       </c>
       <c r="J8" t="inlineStr">
         <is>
-          <t>3666724037004160</t>
+          <t>-424935940825191</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>Gaurav Gupta Live India Tour</t>
+          <t>Mix Open Mic By Shy</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>Anuv Jain - Dastakhat India Tour (Mumbai)DOME, SVP Stadium: MumbaiConcerts₹ 2500 onwardsAnuv Jain - Dastakhat India Tour (Mumbai)CALVIN HARRIS - Live in MumbaiInfinity Bay: MumbaiConcerts₹ 3000 onwardsCALVIN HARRIS - Live in MumbaiBhajan Clubbing - The New Wave of DevotionRangasharda Auditorium: MumbaiConcerts₹ 299 onwardsBhajan Clubbing - The New Wave of DevotionGaurav Gupta Live - India TourFine Arts Society (Sivaswamy Auditorium): ChemburStand up Comedy₹ 799 onwardsGaurav Gupta Live - India Tour</t>
+          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -877,7 +877,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/gaurav-gupta-live-india-tour/ET00358468</t>
+          <t>https://in.bookmyshow.com/events/mix-open-mic-by-shy/ET00408516?webview=true</t>
         </is>
       </c>
       <c r="G9" t="inlineStr">
@@ -892,24 +892,24 @@
       </c>
       <c r="I9" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:45</t>
+          <t>2026-02-03 19:33:51</t>
         </is>
       </c>
       <c r="J9" t="inlineStr">
         <is>
-          <t>8649810493320537</t>
+          <t>1970736146677906</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>Halwa By Amit Tandon</t>
+          <t>The Studio And The Cube</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>Halwa by Amit Tandon-NCPATata Theatre: NCPA.Stand up Comedy₹ 799 onwardsHalwa by Amit Tandon-NCPAJohn Mayer Solo - Live In Mumbai, 2026Mahalaxmi Race Course: MumbaiConcerts₹ 5000 onwardsJohn Mayer Solo - Live In Mumbai, 2026Mahindra Blues Festival 2026Mehboob Studios: Bandra(W)Concerts₹ 4000 onwardsMahindra Blues Festival 2026TOXIC - Abhishek Upmanyu LiveSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 799 onwardsTOXIC - Abhishek Upmanyu Live</t>
+          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
@@ -929,7 +929,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/halwa-by-amit-tandon/ET00478732</t>
+          <t>https://in.bookmyshow.com/events/the-studio-and-the-cube/ET00355397?webview=true</t>
         </is>
       </c>
       <c r="G10" t="inlineStr">
@@ -944,24 +944,24 @@
       </c>
       <c r="I10" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:45</t>
+          <t>2026-02-03 19:33:51</t>
         </is>
       </c>
       <c r="J10" t="inlineStr">
         <is>
-          <t>-652733870842175</t>
+          <t>-470296154214087</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>John Mayer Solo Live In Mumbai 2026</t>
+          <t>Ncpa Upcoming Events</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>Halwa by Amit Tandon-NCPATata Theatre: NCPA.Stand up Comedy₹ 799 onwardsHalwa by Amit Tandon-NCPAJohn Mayer Solo - Live In Mumbai, 2026Mahalaxmi Race Course: MumbaiConcerts₹ 5000 onwardsJohn Mayer Solo - Live In Mumbai, 2026Mahindra Blues Festival 2026Mehboob Studios: Bandra(W)Concerts₹ 4000 onwardsMahindra Blues Festival 2026TOXIC - Abhishek Upmanyu LiveSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 799 onwardsTOXIC - Abhishek Upmanyu Live</t>
+          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -981,7 +981,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/john-mayer-solo-live-in-mumbai-2026/ET00464841</t>
+          <t>https://in.bookmyshow.com/events/ncpa-upcoming-events/ET00305288?webview=true</t>
         </is>
       </c>
       <c r="G11" t="inlineStr">
@@ -996,24 +996,24 @@
       </c>
       <c r="I11" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:45</t>
+          <t>2026-02-03 19:33:51</t>
         </is>
       </c>
       <c r="J11" t="inlineStr">
         <is>
-          <t>1830344615170119</t>
+          <t>8057069907423056</t>
         </is>
       </c>
     </row>
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>Mahindra Blues Festival 2026</t>
+          <t>Vipul Goyal Unleashed</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>Halwa by Amit Tandon-NCPATata Theatre: NCPA.Stand up Comedy₹ 799 onwardsHalwa by Amit Tandon-NCPAJohn Mayer Solo - Live In Mumbai, 2026Mahalaxmi Race Course: MumbaiConcerts₹ 5000 onwardsJohn Mayer Solo - Live In Mumbai, 2026Mahindra Blues Festival 2026Mehboob Studios: Bandra(W)Concerts₹ 4000 onwardsMahindra Blues Festival 2026TOXIC - Abhishek Upmanyu LiveSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 799 onwardsTOXIC - Abhishek Upmanyu Live</t>
+          <t>Thats So Viraj - With Friends A Live Comedy ShowShanmukhananda Hall: MumbaiStand up Comedy₹ 499 onwardsThats So Viraj - With Friends A Live Comedy ShowSounds Good FestivalNesco Center - Goregaon: MumbaiConcerts₹ 999 onwardsSounds Good FestivalLata Mangeshkar ji &amp; R.D. Burman showPrabodhankar Thackeray Audi: Borivali(W)Concerts₹ 200 onwardsLata Mangeshkar ji &amp; R.D. Burman showVIPUL GOYAL UNLEASHEDThe Habitat: MumbaiStand up Comedy₹ 999 onwardsVIPUL GOYAL UNLEASHED</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -1033,7 +1033,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/mahindra-blues-festival-2026/ET00468903</t>
+          <t>https://in.bookmyshow.com/events/vipul-goyal-unleashed/ET00431496</t>
         </is>
       </c>
       <c r="G12" t="inlineStr">
@@ -1048,24 +1048,24 @@
       </c>
       <c r="I12" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:46</t>
+          <t>2026-02-03 19:33:51</t>
         </is>
       </c>
       <c r="J12" t="inlineStr">
         <is>
-          <t>8047608815574611</t>
+          <t>3435355020067613</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>Toxic Abhishek Upmanyu Live</t>
+          <t>Sounds Good Festival</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>Halwa by Amit Tandon-NCPATata Theatre: NCPA.Stand up Comedy₹ 799 onwardsHalwa by Amit Tandon-NCPAJohn Mayer Solo - Live In Mumbai, 2026Mahalaxmi Race Course: MumbaiConcerts₹ 5000 onwardsJohn Mayer Solo - Live In Mumbai, 2026Mahindra Blues Festival 2026Mehboob Studios: Bandra(W)Concerts₹ 4000 onwardsMahindra Blues Festival 2026TOXIC - Abhishek Upmanyu LiveSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 799 onwardsTOXIC - Abhishek Upmanyu Live</t>
+          <t>Thats So Viraj - With Friends A Live Comedy ShowShanmukhananda Hall: MumbaiStand up Comedy₹ 499 onwardsThats So Viraj - With Friends A Live Comedy ShowSounds Good FestivalNesco Center - Goregaon: MumbaiConcerts₹ 999 onwardsSounds Good FestivalLata Mangeshkar ji &amp; R.D. Burman showPrabodhankar Thackeray Audi: Borivali(W)Concerts₹ 200 onwardsLata Mangeshkar ji &amp; R.D. Burman showVIPUL GOYAL UNLEASHEDThe Habitat: MumbaiStand up Comedy₹ 999 onwardsVIPUL GOYAL UNLEASHED</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -1085,7 +1085,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/toxic-abhishek-upmanyu-live/ET00409716</t>
+          <t>https://in.bookmyshow.com/events/sounds-good-festival/ET00483217</t>
         </is>
       </c>
       <c r="G13" t="inlineStr">
@@ -1100,24 +1100,24 @@
       </c>
       <c r="I13" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:46</t>
+          <t>2026-02-03 19:33:50</t>
         </is>
       </c>
       <c r="J13" t="inlineStr">
         <is>
-          <t>-875818091617151</t>
+          <t>-813726566592449</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>Main Shayar Toh Nahi Manhar Seth</t>
+          <t>Thats So Viraj With Friends A Live Comedy Show</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>Main Shayar Toh Nahi- Manhar SethHotel Rang Sharda: MumbaiStand up Comedy₹ 499 onwardsMain Shayar Toh Nahi- Manhar SethSpoken Fest Mumbai 2026Jio World Garden, BKC: MumbaiSpoken Word₹ 999 onwardsSpoken Fest Mumbai 2026Sanam India Tour - MumbaiSouth Sky, Jio World Drive: MumbaiConcerts₹ 2999 onwardsSanam India Tour - MumbaiRough Jokes ft. Amit Tandon: KCCKhar Comedy Club: MumbaiStand up Comedy₹ 499Rough Jokes ft. Amit Tandon: KCC</t>
+          <t>Thats So Viraj - With Friends A Live Comedy ShowShanmukhananda Hall: MumbaiStand up Comedy₹ 499 onwardsThats So Viraj - With Friends A Live Comedy ShowSounds Good FestivalNesco Center - Goregaon: MumbaiConcerts₹ 999 onwardsSounds Good FestivalLata Mangeshkar ji &amp; R.D. Burman showPrabodhankar Thackeray Audi: Borivali(W)Concerts₹ 200 onwardsLata Mangeshkar ji &amp; R.D. Burman showVIPUL GOYAL UNLEASHEDThe Habitat: MumbaiStand up Comedy₹ 999 onwardsVIPUL GOYAL UNLEASHED</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -1137,7 +1137,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/main-shayar-toh-nahi-manhar-seth/ET00469851</t>
+          <t>https://in.bookmyshow.com/events/thats-so-viraj-with-friends-a-live-comedy-show/ET00482495</t>
         </is>
       </c>
       <c r="G14" t="inlineStr">
@@ -1152,24 +1152,24 @@
       </c>
       <c r="I14" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:46</t>
+          <t>2026-02-03 19:33:50</t>
         </is>
       </c>
       <c r="J14" t="inlineStr">
         <is>
-          <t>5909782130821593</t>
+          <t>1253124737492114</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>Spoken Fest Mumbai 2026</t>
+          <t>Lata Mangeshkar Ji R D Burman Show</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>Main Shayar Toh Nahi- Manhar SethHotel Rang Sharda: MumbaiStand up Comedy₹ 499 onwardsMain Shayar Toh Nahi- Manhar SethSpoken Fest Mumbai 2026Jio World Garden, BKC: MumbaiSpoken Word₹ 999 onwardsSpoken Fest Mumbai 2026Sanam India Tour - MumbaiSouth Sky, Jio World Drive: MumbaiConcerts₹ 2999 onwardsSanam India Tour - MumbaiRough Jokes ft. Amit Tandon: KCCKhar Comedy Club: MumbaiStand up Comedy₹ 499Rough Jokes ft. Amit Tandon: KCC</t>
+          <t>Thats So Viraj - With Friends A Live Comedy ShowShanmukhananda Hall: MumbaiStand up Comedy₹ 499 onwardsThats So Viraj - With Friends A Live Comedy ShowSounds Good FestivalNesco Center - Goregaon: MumbaiConcerts₹ 999 onwardsSounds Good FestivalLata Mangeshkar ji &amp; R.D. Burman showPrabodhankar Thackeray Audi: Borivali(W)Concerts₹ 200 onwardsLata Mangeshkar ji &amp; R.D. Burman showVIPUL GOYAL UNLEASHEDThe Habitat: MumbaiStand up Comedy₹ 999 onwardsVIPUL GOYAL UNLEASHED</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -1189,7 +1189,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/spoken-fest-mumbai-2026/ET00458598</t>
+          <t>https://in.bookmyshow.com/events/lata-mangeshkar-ji-r-d-burman-show/ET00472998</t>
         </is>
       </c>
       <c r="G15" t="inlineStr">
@@ -1204,24 +1204,24 @@
       </c>
       <c r="I15" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:46</t>
+          <t>2026-02-03 19:33:50</t>
         </is>
       </c>
       <c r="J15" t="inlineStr">
         <is>
-          <t>8178184370217172</t>
+          <t>-220083242171281</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>Sanam India Tour Mumbai</t>
+          <t>Aawara Hoon</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>Main Shayar Toh Nahi- Manhar SethHotel Rang Sharda: MumbaiStand up Comedy₹ 499 onwardsMain Shayar Toh Nahi- Manhar SethSpoken Fest Mumbai 2026Jio World Garden, BKC: MumbaiSpoken Word₹ 999 onwardsSpoken Fest Mumbai 2026Sanam India Tour - MumbaiSouth Sky, Jio World Drive: MumbaiConcerts₹ 2999 onwardsSanam India Tour - MumbaiRough Jokes ft. Amit Tandon: KCCKhar Comedy Club: MumbaiStand up Comedy₹ 499Rough Jokes ft. Amit Tandon: KCC</t>
+          <t>Manoj Muntashir's Krishna - Radha Se Ranbhumi TakThe Grand Theatre, NMACCConcerts₹ 2500 onwardsManoj Muntashir's Krishna - Radha Se Ranbhumi TakLetters to Lata Didi by Shreya GhoshalJio World Garden, BKC: MumbaiConcerts₹ 2999 onwardsLetters to Lata Didi by Shreya GhoshalHori Ke Rang - Compositions on HoriTata Theatre: NCPA.Concerts₹ 500 onwardsHori Ke Rang - Compositions on HoriAAWARA HOONRam Ganesh Gadkari Rangayatan: ThaneConcerts₹ 300 onwardsAAWARA HOON</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
@@ -1241,7 +1241,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/sanam-india-tour-mumbai/ET00466356</t>
+          <t>https://in.bookmyshow.com/events/aawara-hoon/ET00421569</t>
         </is>
       </c>
       <c r="G16" t="inlineStr">
@@ -1256,24 +1256,24 @@
       </c>
       <c r="I16" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:47</t>
+          <t>2026-02-03 19:33:49</t>
         </is>
       </c>
       <c r="J16" t="inlineStr">
         <is>
-          <t>-863857139495437</t>
+          <t>8991187371837192</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>Amit Tondon Live Kcc</t>
+          <t>Hori Ke Rang Traditional Compositions On Hori</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>Main Shayar Toh Nahi- Manhar SethHotel Rang Sharda: MumbaiStand up Comedy₹ 499 onwardsMain Shayar Toh Nahi- Manhar SethSpoken Fest Mumbai 2026Jio World Garden, BKC: MumbaiSpoken Word₹ 999 onwardsSpoken Fest Mumbai 2026Sanam India Tour - MumbaiSouth Sky, Jio World Drive: MumbaiConcerts₹ 2999 onwardsSanam India Tour - MumbaiRough Jokes ft. Amit Tandon: KCCKhar Comedy Club: MumbaiStand up Comedy₹ 499Rough Jokes ft. Amit Tandon: KCC</t>
+          <t>Manoj Muntashir's Krishna - Radha Se Ranbhumi TakThe Grand Theatre, NMACCConcerts₹ 2500 onwardsManoj Muntashir's Krishna - Radha Se Ranbhumi TakLetters to Lata Didi by Shreya GhoshalJio World Garden, BKC: MumbaiConcerts₹ 2999 onwardsLetters to Lata Didi by Shreya GhoshalHori Ke Rang - Compositions on HoriTata Theatre: NCPA.Concerts₹ 500 onwardsHori Ke Rang - Compositions on HoriAAWARA HOONRam Ganesh Gadkari Rangayatan: ThaneConcerts₹ 300 onwardsAAWARA HOON</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
@@ -1293,7 +1293,7 @@
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/amit-tondon-live-kcc/ET00473247</t>
+          <t>https://in.bookmyshow.com/events/hori-ke-rang-traditional-compositions-on-hori/ET00479306</t>
         </is>
       </c>
       <c r="G17" t="inlineStr">
@@ -1308,24 +1308,24 @@
       </c>
       <c r="I17" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:47</t>
+          <t>2026-02-03 19:33:49</t>
         </is>
       </c>
       <c r="J17" t="inlineStr">
         <is>
-          <t>7213896662123453</t>
+          <t>-738906713022258</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
-          <t>Manoj Muntashir S Krishna Radha Se Ranbhumi Tak</t>
+          <t>Letters To Lata Didi By Shreya Ghoshal</t>
         </is>
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>Manoj Muntashir's Krishna - Radha Se Ranbhumi TakThe Grand Theatre, NMACCConcerts₹ 2500 onwardsManoj Muntashir's Krishna - Radha Se Ranbhumi TakLetters to Lata Didi by Shreya GhoshalJio World Garden, BKC: MumbaiConcerts₹ 2999 onwardsLetters to Lata Didi by Shreya GhoshalSama'a: Festival of Sufi Music - Day 3Tata Theatre: NCPAConcerts₹ 500 onwardsSama'a: Festival of Sufi Music - Day 3Doug Aitken: UNDER THE SUNArt House, Nita Mukesh Ambani Cultural CentreArt Exhibitions₹ 250 onwardsDoug Aitken: UNDER THE SUN</t>
+          <t>Manoj Muntashir's Krishna - Radha Se Ranbhumi TakThe Grand Theatre, NMACCConcerts₹ 2500 onwardsManoj Muntashir's Krishna - Radha Se Ranbhumi TakLetters to Lata Didi by Shreya GhoshalJio World Garden, BKC: MumbaiConcerts₹ 2999 onwardsLetters to Lata Didi by Shreya GhoshalHori Ke Rang - Compositions on HoriTata Theatre: NCPA.Concerts₹ 500 onwardsHori Ke Rang - Compositions on HoriAAWARA HOONRam Ganesh Gadkari Rangayatan: ThaneConcerts₹ 300 onwardsAAWARA HOON</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
@@ -1345,7 +1345,7 @@
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/manoj-muntashir-s-krishna-radha-se-ranbhumi-tak/ET00482458</t>
+          <t>https://in.bookmyshow.com/events/letters-to-lata-didi-by-shreya-ghoshal/ET00474204</t>
         </is>
       </c>
       <c r="G18" t="inlineStr">
@@ -1360,24 +1360,24 @@
       </c>
       <c r="I18" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:47</t>
+          <t>2026-02-03 19:33:49</t>
         </is>
       </c>
       <c r="J18" t="inlineStr">
         <is>
-          <t>-300658533514382</t>
+          <t>5347043071395239</t>
         </is>
       </c>
     </row>
     <row r="19">
       <c r="A19" t="inlineStr">
         <is>
-          <t>Letters To Lata Didi By Shreya Ghoshal</t>
+          <t>Manoj Muntashir S Krishna Radha Se Ranbhumi Tak</t>
         </is>
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>Manoj Muntashir's Krishna - Radha Se Ranbhumi TakThe Grand Theatre, NMACCConcerts₹ 2500 onwardsManoj Muntashir's Krishna - Radha Se Ranbhumi TakLetters to Lata Didi by Shreya GhoshalJio World Garden, BKC: MumbaiConcerts₹ 2999 onwardsLetters to Lata Didi by Shreya GhoshalSama'a: Festival of Sufi Music - Day 3Tata Theatre: NCPAConcerts₹ 500 onwardsSama'a: Festival of Sufi Music - Day 3Doug Aitken: UNDER THE SUNArt House, Nita Mukesh Ambani Cultural CentreArt Exhibitions₹ 250 onwardsDoug Aitken: UNDER THE SUN</t>
+          <t>Manoj Muntashir's Krishna - Radha Se Ranbhumi TakThe Grand Theatre, NMACCConcerts₹ 2500 onwardsManoj Muntashir's Krishna - Radha Se Ranbhumi TakLetters to Lata Didi by Shreya GhoshalJio World Garden, BKC: MumbaiConcerts₹ 2999 onwardsLetters to Lata Didi by Shreya GhoshalHori Ke Rang - Compositions on HoriTata Theatre: NCPA.Concerts₹ 500 onwardsHori Ke Rang - Compositions on HoriAAWARA HOONRam Ganesh Gadkari Rangayatan: ThaneConcerts₹ 300 onwardsAAWARA HOON</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
@@ -1397,7 +1397,7 @@
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/letters-to-lata-didi-by-shreya-ghoshal/ET00474204</t>
+          <t>https://in.bookmyshow.com/events/manoj-muntashir-s-krishna-radha-se-ranbhumi-tak/ET00482458</t>
         </is>
       </c>
       <c r="G19" t="inlineStr">
@@ -1412,24 +1412,24 @@
       </c>
       <c r="I19" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:48</t>
+          <t>2026-02-03 19:33:48</t>
         </is>
       </c>
       <c r="J19" t="inlineStr">
         <is>
-          <t>8311854138617698</t>
+          <t>-770600238694201</t>
         </is>
       </c>
     </row>
     <row r="20">
       <c r="A20" t="inlineStr">
         <is>
-          <t>Sama A Festival Of Sufi Music Day 3</t>
+          <t>Amit Tondon Live Kcc</t>
         </is>
       </c>
       <c r="B20" t="inlineStr">
         <is>
-          <t>Manoj Muntashir's Krishna - Radha Se Ranbhumi TakThe Grand Theatre, NMACCConcerts₹ 2500 onwardsManoj Muntashir's Krishna - Radha Se Ranbhumi TakLetters to Lata Didi by Shreya GhoshalJio World Garden, BKC: MumbaiConcerts₹ 2999 onwardsLetters to Lata Didi by Shreya GhoshalSama'a: Festival of Sufi Music - Day 3Tata Theatre: NCPAConcerts₹ 500 onwardsSama'a: Festival of Sufi Music - Day 3Doug Aitken: UNDER THE SUNArt House, Nita Mukesh Ambani Cultural CentreArt Exhibitions₹ 250 onwardsDoug Aitken: UNDER THE SUN</t>
+          <t>Main Shayar Toh Nahi- Manhar SethHotel Rang Sharda: MumbaiStand up Comedy₹ 499 onwardsMain Shayar Toh Nahi- Manhar SethSpoken Fest Mumbai 2026Jio World Garden, BKC: MumbaiSpoken Word₹ 999 onwardsSpoken Fest Mumbai 2026Sanam India Tour - MumbaiSouth Sky, Jio World Drive: MumbaiConcerts₹ 2999 onwardsSanam India Tour - MumbaiRough Jokes ft. Amit Tandon: KCCKhar Comedy Club: MumbaiStand up Comedy₹ 499Rough Jokes ft. Amit Tandon: KCC</t>
         </is>
       </c>
       <c r="C20" t="inlineStr">
@@ -1449,7 +1449,7 @@
       </c>
       <c r="F20" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/sama-a-festival-of-sufi-music-day-3/ET00480910</t>
+          <t>https://in.bookmyshow.com/events/amit-tondon-live-kcc/ET00473247</t>
         </is>
       </c>
       <c r="G20" t="inlineStr">
@@ -1464,24 +1464,24 @@
       </c>
       <c r="I20" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:48</t>
+          <t>2026-02-03 19:33:48</t>
         </is>
       </c>
       <c r="J20" t="inlineStr">
         <is>
-          <t>-462539575990560</t>
+          <t>-599079955836177</t>
         </is>
       </c>
     </row>
     <row r="21">
       <c r="A21" t="inlineStr">
         <is>
-          <t>Doug Aitken Under The Sun</t>
+          <t>Sanam India Tour Mumbai</t>
         </is>
       </c>
       <c r="B21" t="inlineStr">
         <is>
-          <t>Manoj Muntashir's Krishna - Radha Se Ranbhumi TakThe Grand Theatre, NMACCConcerts₹ 2500 onwardsManoj Muntashir's Krishna - Radha Se Ranbhumi TakLetters to Lata Didi by Shreya GhoshalJio World Garden, BKC: MumbaiConcerts₹ 2999 onwardsLetters to Lata Didi by Shreya GhoshalSama'a: Festival of Sufi Music - Day 3Tata Theatre: NCPAConcerts₹ 500 onwardsSama'a: Festival of Sufi Music - Day 3Doug Aitken: UNDER THE SUNArt House, Nita Mukesh Ambani Cultural CentreArt Exhibitions₹ 250 onwardsDoug Aitken: UNDER THE SUN</t>
+          <t>Main Shayar Toh Nahi- Manhar SethHotel Rang Sharda: MumbaiStand up Comedy₹ 499 onwardsMain Shayar Toh Nahi- Manhar SethSpoken Fest Mumbai 2026Jio World Garden, BKC: MumbaiSpoken Word₹ 999 onwardsSpoken Fest Mumbai 2026Sanam India Tour - MumbaiSouth Sky, Jio World Drive: MumbaiConcerts₹ 2999 onwardsSanam India Tour - MumbaiRough Jokes ft. Amit Tandon: KCCKhar Comedy Club: MumbaiStand up Comedy₹ 499Rough Jokes ft. Amit Tandon: KCC</t>
         </is>
       </c>
       <c r="C21" t="inlineStr">
@@ -1501,7 +1501,7 @@
       </c>
       <c r="F21" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/doug-aitken-under-the-sun/ET00469533</t>
+          <t>https://in.bookmyshow.com/events/sanam-india-tour-mumbai/ET00466356</t>
         </is>
       </c>
       <c r="G21" t="inlineStr">
@@ -1516,24 +1516,24 @@
       </c>
       <c r="I21" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:48</t>
+          <t>2026-02-03 19:33:48</t>
         </is>
       </c>
       <c r="J21" t="inlineStr">
         <is>
-          <t>9132104223511360</t>
+          <t>1876288917409645</t>
         </is>
       </c>
     </row>
     <row r="22">
       <c r="A22" t="inlineStr">
         <is>
-          <t>Ncpa Upcoming Events</t>
+          <t>Spoken Fest Mumbai 2026</t>
         </is>
       </c>
       <c r="B22" t="inlineStr">
         <is>
-          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
+          <t>Main Shayar Toh Nahi- Manhar SethHotel Rang Sharda: MumbaiStand up Comedy₹ 499 onwardsMain Shayar Toh Nahi- Manhar SethSpoken Fest Mumbai 2026Jio World Garden, BKC: MumbaiSpoken Word₹ 999 onwardsSpoken Fest Mumbai 2026Sanam India Tour - MumbaiSouth Sky, Jio World Drive: MumbaiConcerts₹ 2999 onwardsSanam India Tour - MumbaiRough Jokes ft. Amit Tandon: KCCKhar Comedy Club: MumbaiStand up Comedy₹ 499Rough Jokes ft. Amit Tandon: KCC</t>
         </is>
       </c>
       <c r="C22" t="inlineStr">
@@ -1553,7 +1553,7 @@
       </c>
       <c r="F22" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/ncpa-upcoming-events/ET00305288?webview=true</t>
+          <t>https://in.bookmyshow.com/events/spoken-fest-mumbai-2026/ET00458598</t>
         </is>
       </c>
       <c r="G22" t="inlineStr">
@@ -1568,24 +1568,24 @@
       </c>
       <c r="I22" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:49</t>
+          <t>2026-02-03 19:33:48</t>
         </is>
       </c>
       <c r="J22" t="inlineStr">
         <is>
-          <t>9113988627658034</t>
+          <t>9691241088840277</t>
         </is>
       </c>
     </row>
     <row r="23">
       <c r="A23" t="inlineStr">
         <is>
-          <t>The Studio And The Cube</t>
+          <t>Main Shayar Toh Nahi Manhar Seth</t>
         </is>
       </c>
       <c r="B23" t="inlineStr">
         <is>
-          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
+          <t>Main Shayar Toh Nahi- Manhar SethHotel Rang Sharda: MumbaiStand up Comedy₹ 499 onwardsMain Shayar Toh Nahi- Manhar SethSpoken Fest Mumbai 2026Jio World Garden, BKC: MumbaiSpoken Word₹ 999 onwardsSpoken Fest Mumbai 2026Sanam India Tour - MumbaiSouth Sky, Jio World Drive: MumbaiConcerts₹ 2999 onwardsSanam India Tour - MumbaiRough Jokes ft. Amit Tandon: KCCKhar Comedy Club: MumbaiStand up Comedy₹ 499Rough Jokes ft. Amit Tandon: KCC</t>
         </is>
       </c>
       <c r="C23" t="inlineStr">
@@ -1605,7 +1605,7 @@
       </c>
       <c r="F23" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/the-studio-and-the-cube/ET00355397?webview=true</t>
+          <t>https://in.bookmyshow.com/events/main-shayar-toh-nahi-manhar-seth/ET00469851</t>
         </is>
       </c>
       <c r="G23" t="inlineStr">
@@ -1620,24 +1620,24 @@
       </c>
       <c r="I23" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:49</t>
+          <t>2026-02-03 19:33:47</t>
         </is>
       </c>
       <c r="J23" t="inlineStr">
         <is>
-          <t>7713217154567214</t>
+          <t>8617276307077354</t>
         </is>
       </c>
     </row>
     <row r="24">
       <c r="A24" t="inlineStr">
         <is>
-          <t>Mix Open Mic By Shy</t>
+          <t>Toxic Abhishek Upmanyu Live</t>
         </is>
       </c>
       <c r="B24" t="inlineStr">
         <is>
-          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
+          <t>Bhajan Clubbing - The New Wave of DevotionRangasharda Auditorium: MumbaiConcerts₹ 299 onwardsBhajan Clubbing - The New Wave of DevotionGaurav Gupta Live - India TourFine Arts Society (Sivaswamy Auditorium): ChemburStand up Comedy₹ 799 onwardsGaurav Gupta Live - India TourHalwa by Amit Tandon-NCPATata Theatre: NCPA.Stand up Comedy₹ 799 onwardsHalwa by Amit Tandon-NCPATOXIC - Abhishek Upmanyu LiveSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 799 onwardsTOXIC - Abhishek Upmanyu Live</t>
         </is>
       </c>
       <c r="C24" t="inlineStr">
@@ -1657,7 +1657,7 @@
       </c>
       <c r="F24" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/mix-open-mic-by-shy/ET00408516?webview=true</t>
+          <t>https://in.bookmyshow.com/events/toxic-abhishek-upmanyu-live/ET00409716</t>
         </is>
       </c>
       <c r="G24" t="inlineStr">
@@ -1672,24 +1672,24 @@
       </c>
       <c r="I24" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:49</t>
+          <t>2026-02-03 19:33:47</t>
         </is>
       </c>
       <c r="J24" t="inlineStr">
         <is>
-          <t>3834458038488217</t>
+          <t>1906025406297492</t>
         </is>
       </c>
     </row>
     <row r="25">
       <c r="A25" t="inlineStr">
         <is>
-          <t>Sunburn Upcoming Events</t>
+          <t>Halwa By Amit Tandon</t>
         </is>
       </c>
       <c r="B25" t="inlineStr">
         <is>
-          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
+          <t>Bhajan Clubbing - The New Wave of DevotionRangasharda Auditorium: MumbaiConcerts₹ 299 onwardsBhajan Clubbing - The New Wave of DevotionGaurav Gupta Live - India TourFine Arts Society (Sivaswamy Auditorium): ChemburStand up Comedy₹ 799 onwardsGaurav Gupta Live - India TourHalwa by Amit Tandon-NCPATata Theatre: NCPA.Stand up Comedy₹ 799 onwardsHalwa by Amit Tandon-NCPATOXIC - Abhishek Upmanyu LiveSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 799 onwardsTOXIC - Abhishek Upmanyu Live</t>
         </is>
       </c>
       <c r="C25" t="inlineStr">
@@ -1709,7 +1709,7 @@
       </c>
       <c r="F25" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/sunburn-upcoming-events/ET00463644?webview=true</t>
+          <t>https://in.bookmyshow.com/events/halwa-by-amit-tandon/ET00478732</t>
         </is>
       </c>
       <c r="G25" t="inlineStr">
@@ -1724,24 +1724,24 @@
       </c>
       <c r="I25" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:49</t>
+          <t>2026-02-03 19:33:47</t>
         </is>
       </c>
       <c r="J25" t="inlineStr">
         <is>
-          <t>-123678172414039</t>
+          <t>-189384428446319</t>
         </is>
       </c>
     </row>
     <row r="26">
       <c r="A26" t="inlineStr">
         <is>
-          <t>Laptop Dj Workshop</t>
+          <t>Gaurav Gupta Live India Tour</t>
         </is>
       </c>
       <c r="B26" t="inlineStr">
         <is>
-          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
+          <t>Bhajan Clubbing - The New Wave of DevotionRangasharda Auditorium: MumbaiConcerts₹ 299 onwardsBhajan Clubbing - The New Wave of DevotionGaurav Gupta Live - India TourFine Arts Society (Sivaswamy Auditorium): ChemburStand up Comedy₹ 799 onwardsGaurav Gupta Live - India TourHalwa by Amit Tandon-NCPATata Theatre: NCPA.Stand up Comedy₹ 799 onwardsHalwa by Amit Tandon-NCPATOXIC - Abhishek Upmanyu LiveSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 799 onwardsTOXIC - Abhishek Upmanyu Live</t>
         </is>
       </c>
       <c r="C26" t="inlineStr">
@@ -1761,7 +1761,7 @@
       </c>
       <c r="F26" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/laptop-dj-workshop/ET00425192?webview=true</t>
+          <t>https://in.bookmyshow.com/events/gaurav-gupta-live-india-tour/ET00358468</t>
         </is>
       </c>
       <c r="G26" t="inlineStr">
@@ -1776,24 +1776,24 @@
       </c>
       <c r="I26" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:50</t>
+          <t>2026-02-03 19:33:46</t>
         </is>
       </c>
       <c r="J26" t="inlineStr">
         <is>
-          <t>1770852189171252</t>
+          <t>-119042637683662</t>
         </is>
       </c>
     </row>
     <row r="27">
       <c r="A27" t="inlineStr">
         <is>
-          <t>Pookie Jams The Premium Jamming Experience</t>
+          <t>Bhajan Clubbing The New Wave Of Devotion</t>
         </is>
       </c>
       <c r="B27" t="inlineStr">
         <is>
-          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
+          <t>Bhajan Clubbing - The New Wave of DevotionRangasharda Auditorium: MumbaiConcerts₹ 299 onwardsBhajan Clubbing - The New Wave of DevotionGaurav Gupta Live - India TourFine Arts Society (Sivaswamy Auditorium): ChemburStand up Comedy₹ 799 onwardsGaurav Gupta Live - India TourHalwa by Amit Tandon-NCPATata Theatre: NCPA.Stand up Comedy₹ 799 onwardsHalwa by Amit Tandon-NCPATOXIC - Abhishek Upmanyu LiveSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 799 onwardsTOXIC - Abhishek Upmanyu Live</t>
         </is>
       </c>
       <c r="C27" t="inlineStr">
@@ -1813,7 +1813,7 @@
       </c>
       <c r="F27" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/pookie-jams-the-premium-jamming-experience/ET00461172?webview=true</t>
+          <t>https://in.bookmyshow.com/events/bhajan-clubbing-the-new-wave-of-devotion/ET00481773</t>
         </is>
       </c>
       <c r="G27" t="inlineStr">
@@ -1828,24 +1828,24 @@
       </c>
       <c r="I27" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:50</t>
+          <t>2026-02-03 19:33:46</t>
         </is>
       </c>
       <c r="J27" t="inlineStr">
         <is>
-          <t>-122199657807012</t>
+          <t>-685129594106800</t>
         </is>
       </c>
     </row>
     <row r="28">
       <c r="A28" t="inlineStr">
         <is>
-          <t>Vocal Workshop</t>
+          <t>Anuv Jain Dastakhat India Tour Mumbai</t>
         </is>
       </c>
       <c r="B28" t="inlineStr">
         <is>
-          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
+          <t>Chhoti Soch - A Standup Solo By Shubham PujariThe Habitat: MumbaiStand up Comedy₹ 399 onwardsChhoti Soch - A Standup Solo By Shubham PujariTonight In Juhu - A Live Standup Comedy ShowThe J Spot, Juhu: MumbaiStand up Comedy₹ 349 onwardsTonight In Juhu - A Live Standup Comedy ShowDaily Ka Kaam Hai By Aakash Gupta - MumbaiSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 599 onwardsDaily Ka Kaam Hai By Aakash Gupta - MumbaiAnuv Jain - Dastakhat India Tour (Mumbai)DOME, SVP Stadium: MumbaiConcerts₹ 2500 onwardsAnuv Jain - Dastakhat India Tour (Mumbai)</t>
         </is>
       </c>
       <c r="C28" t="inlineStr">
@@ -1865,7 +1865,7 @@
       </c>
       <c r="F28" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/vocal-workshop/ET00393019?webview=true</t>
+          <t>https://in.bookmyshow.com/events/anuv-jain-dastakhat-india-tour-mumbai/ET00470487</t>
         </is>
       </c>
       <c r="G28" t="inlineStr">
@@ -1880,24 +1880,24 @@
       </c>
       <c r="I28" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:50</t>
+          <t>2026-02-03 19:33:46</t>
         </is>
       </c>
       <c r="J28" t="inlineStr">
         <is>
-          <t>1824526730218450</t>
+          <t>3982553524420707</t>
         </is>
       </c>
     </row>
     <row r="29">
       <c r="A29" t="inlineStr">
         <is>
-          <t>The Soi Spring 2026 Season</t>
+          <t>Tonight In Juhu</t>
         </is>
       </c>
       <c r="B29" t="inlineStr">
         <is>
-          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
+          <t>Chhoti Soch - A Standup Solo By Shubham PujariThe Habitat: MumbaiStand up Comedy₹ 399 onwardsChhoti Soch - A Standup Solo By Shubham PujariTonight In Juhu - A Live Standup Comedy ShowThe J Spot, Juhu: MumbaiStand up Comedy₹ 349 onwardsTonight In Juhu - A Live Standup Comedy ShowDaily Ka Kaam Hai By Aakash Gupta - MumbaiSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 599 onwardsDaily Ka Kaam Hai By Aakash Gupta - MumbaiAnuv Jain - Dastakhat India Tour (Mumbai)DOME, SVP Stadium: MumbaiConcerts₹ 2500 onwardsAnuv Jain - Dastakhat India Tour (Mumbai)</t>
         </is>
       </c>
       <c r="C29" t="inlineStr">
@@ -1917,7 +1917,7 @@
       </c>
       <c r="F29" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/the-soi-spring-2026-season/ET00473378?webview=true</t>
+          <t>https://in.bookmyshow.com/events/tonight-in-juhu/ET00469058</t>
         </is>
       </c>
       <c r="G29" t="inlineStr">
@@ -1932,24 +1932,24 @@
       </c>
       <c r="I29" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:51</t>
+          <t>2026-02-03 19:33:45</t>
         </is>
       </c>
       <c r="J29" t="inlineStr">
         <is>
-          <t>9209435914068632</t>
+          <t>1044682619402221</t>
         </is>
       </c>
     </row>
     <row r="30">
       <c r="A30" t="inlineStr">
         <is>
-          <t>The Dj Blues 2 And 1 Salsa Elementary Workshop</t>
+          <t>Daily Ka Kaam Hai By Aakash Gupta Mumbai</t>
         </is>
       </c>
       <c r="B30" t="inlineStr">
         <is>
-          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
+          <t>Chhoti Soch - A Standup Solo By Shubham PujariThe Habitat: MumbaiStand up Comedy₹ 399 onwardsChhoti Soch - A Standup Solo By Shubham PujariTonight In Juhu - A Live Standup Comedy ShowThe J Spot, Juhu: MumbaiStand up Comedy₹ 349 onwardsTonight In Juhu - A Live Standup Comedy ShowDaily Ka Kaam Hai By Aakash Gupta - MumbaiSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 599 onwardsDaily Ka Kaam Hai By Aakash Gupta - MumbaiAnuv Jain - Dastakhat India Tour (Mumbai)DOME, SVP Stadium: MumbaiConcerts₹ 2500 onwardsAnuv Jain - Dastakhat India Tour (Mumbai)</t>
         </is>
       </c>
       <c r="C30" t="inlineStr">
@@ -1969,7 +1969,7 @@
       </c>
       <c r="F30" t="inlineStr">
         <is>
-          <t>https://in.bookmyshow.com/events/the-dj-blues-2-and-1-salsa-elementary-workshop/ET00482759?webview=true</t>
+          <t>https://in.bookmyshow.com/events/daily-ka-kaam-hai-by-aakash-gupta-mumbai/ET00429299</t>
         </is>
       </c>
       <c r="G30" t="inlineStr">
@@ -1984,65 +1984,1565 @@
       </c>
       <c r="I30" t="inlineStr">
         <is>
-          <t>2026-02-03 18:14:51</t>
+          <t>2026-02-03 19:33:45</t>
         </is>
       </c>
       <c r="J30" t="inlineStr">
         <is>
-          <t>-393889681834392</t>
+          <t>-390327240082061</t>
         </is>
       </c>
     </row>
     <row r="31">
       <c r="A31" t="inlineStr">
         <is>
+          <t>Chhoti Soch A Standup Solo By Shubham Pujari</t>
+        </is>
+      </c>
+      <c r="B31" t="inlineStr">
+        <is>
+          <t>Chhoti Soch - A Standup Solo By Shubham PujariThe Habitat: MumbaiStand up Comedy₹ 399 onwardsChhoti Soch - A Standup Solo By Shubham PujariTonight In Juhu - A Live Standup Comedy ShowThe J Spot, Juhu: MumbaiStand up Comedy₹ 349 onwardsTonight In Juhu - A Live Standup Comedy ShowDaily Ka Kaam Hai By Aakash Gupta - MumbaiSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 599 onwardsDaily Ka Kaam Hai By Aakash Gupta - MumbaiAnuv Jain - Dastakhat India Tour (Mumbai)DOME, SVP Stadium: MumbaiConcerts₹ 2500 onwardsAnuv Jain - Dastakhat India Tour (Mumbai)</t>
+        </is>
+      </c>
+      <c r="C31" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D31" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E31" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F31" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/chhoti-soch-a-standup-solo-by-shubham-pujari/ET00479853</t>
+        </is>
+      </c>
+      <c r="G31" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H31" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I31" t="inlineStr">
+        <is>
+          <t>2026-02-03 19:33:45</t>
+        </is>
+      </c>
+      <c r="J31" t="inlineStr">
+        <is>
+          <t>-586623939302515</t>
+        </is>
+      </c>
+    </row>
+    <row r="32">
+      <c r="A32" t="inlineStr">
+        <is>
           <t>Sama A Festival Of Sufi Music</t>
         </is>
       </c>
-      <c r="B31" t="inlineStr">
+      <c r="B32" t="inlineStr">
         <is>
           <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
         </is>
       </c>
-      <c r="C31" t="inlineStr">
-        <is>
-          <t>Various Venues</t>
-        </is>
-      </c>
-      <c r="D31" t="inlineStr">
-        <is>
-          <t>Mumbai</t>
-        </is>
-      </c>
-      <c r="E31" t="inlineStr">
-        <is>
-          <t>General</t>
-        </is>
-      </c>
-      <c r="F31" t="inlineStr">
+      <c r="C32" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D32" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E32" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F32" t="inlineStr">
         <is>
           <t>https://in.bookmyshow.com/events/sama-a-festival-of-sufi-music/ET00480911?webview=true</t>
         </is>
       </c>
-      <c r="G31" t="inlineStr">
-        <is>
-          <t>BookMyShow</t>
-        </is>
-      </c>
-      <c r="H31" t="inlineStr">
-        <is>
-          <t>Active</t>
-        </is>
-      </c>
-      <c r="I31" t="inlineStr">
+      <c r="G32" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H32" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I32" t="inlineStr">
         <is>
           <t>2026-02-03 18:14:51</t>
         </is>
       </c>
-      <c r="J31" t="inlineStr">
-        <is>
-          <t>-688566512272481</t>
-        </is>
+      <c r="J32" t="n">
+        <v>-688566512272481</v>
+      </c>
+    </row>
+    <row r="33">
+      <c r="A33" t="inlineStr">
+        <is>
+          <t>The Dj Blues 2 And 1 Salsa Elementary Workshop</t>
+        </is>
+      </c>
+      <c r="B33" t="inlineStr">
+        <is>
+          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
+        </is>
+      </c>
+      <c r="C33" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D33" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E33" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F33" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/the-dj-blues-2-and-1-salsa-elementary-workshop/ET00482759?webview=true</t>
+        </is>
+      </c>
+      <c r="G33" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H33" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I33" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:51</t>
+        </is>
+      </c>
+      <c r="J33" t="n">
+        <v>-393889681834392</v>
+      </c>
+    </row>
+    <row r="34">
+      <c r="A34" t="inlineStr">
+        <is>
+          <t>The Soi Spring 2026 Season</t>
+        </is>
+      </c>
+      <c r="B34" t="inlineStr">
+        <is>
+          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
+        </is>
+      </c>
+      <c r="C34" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D34" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E34" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F34" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/the-soi-spring-2026-season/ET00473378?webview=true</t>
+        </is>
+      </c>
+      <c r="G34" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H34" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I34" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:51</t>
+        </is>
+      </c>
+      <c r="J34" t="n">
+        <v>9209435914068632</v>
+      </c>
+    </row>
+    <row r="35">
+      <c r="A35" t="inlineStr">
+        <is>
+          <t>Vocal Workshop</t>
+        </is>
+      </c>
+      <c r="B35" t="inlineStr">
+        <is>
+          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
+        </is>
+      </c>
+      <c r="C35" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D35" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E35" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F35" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/vocal-workshop/ET00393019?webview=true</t>
+        </is>
+      </c>
+      <c r="G35" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H35" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I35" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:50</t>
+        </is>
+      </c>
+      <c r="J35" t="n">
+        <v>1824526730218450</v>
+      </c>
+    </row>
+    <row r="36">
+      <c r="A36" t="inlineStr">
+        <is>
+          <t>Pookie Jams The Premium Jamming Experience</t>
+        </is>
+      </c>
+      <c r="B36" t="inlineStr">
+        <is>
+          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
+        </is>
+      </c>
+      <c r="C36" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D36" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E36" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F36" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/pookie-jams-the-premium-jamming-experience/ET00461172?webview=true</t>
+        </is>
+      </c>
+      <c r="G36" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H36" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I36" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:50</t>
+        </is>
+      </c>
+      <c r="J36" t="n">
+        <v>-122199657807012</v>
+      </c>
+    </row>
+    <row r="37">
+      <c r="A37" t="inlineStr">
+        <is>
+          <t>Laptop Dj Workshop</t>
+        </is>
+      </c>
+      <c r="B37" t="inlineStr">
+        <is>
+          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
+        </is>
+      </c>
+      <c r="C37" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D37" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E37" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F37" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/laptop-dj-workshop/ET00425192?webview=true</t>
+        </is>
+      </c>
+      <c r="G37" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H37" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I37" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:50</t>
+        </is>
+      </c>
+      <c r="J37" t="n">
+        <v>1770852189171252</v>
+      </c>
+    </row>
+    <row r="38">
+      <c r="A38" t="inlineStr">
+        <is>
+          <t>Sunburn Upcoming Events</t>
+        </is>
+      </c>
+      <c r="B38" t="inlineStr">
+        <is>
+          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
+        </is>
+      </c>
+      <c r="C38" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D38" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E38" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F38" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/sunburn-upcoming-events/ET00463644?webview=true</t>
+        </is>
+      </c>
+      <c r="G38" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H38" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I38" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:49</t>
+        </is>
+      </c>
+      <c r="J38" t="n">
+        <v>-123678172414039</v>
+      </c>
+    </row>
+    <row r="39">
+      <c r="A39" t="inlineStr">
+        <is>
+          <t>Mix Open Mic By Shy</t>
+        </is>
+      </c>
+      <c r="B39" t="inlineStr">
+        <is>
+          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
+        </is>
+      </c>
+      <c r="C39" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D39" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E39" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F39" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/mix-open-mic-by-shy/ET00408516?webview=true</t>
+        </is>
+      </c>
+      <c r="G39" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H39" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I39" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:49</t>
+        </is>
+      </c>
+      <c r="J39" t="n">
+        <v>3834458038488217</v>
+      </c>
+    </row>
+    <row r="40">
+      <c r="A40" t="inlineStr">
+        <is>
+          <t>The Studio And The Cube</t>
+        </is>
+      </c>
+      <c r="B40" t="inlineStr">
+        <is>
+          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
+        </is>
+      </c>
+      <c r="C40" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D40" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E40" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F40" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/the-studio-and-the-cube/ET00355397?webview=true</t>
+        </is>
+      </c>
+      <c r="G40" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H40" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I40" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:49</t>
+        </is>
+      </c>
+      <c r="J40" t="n">
+        <v>7713217154567214</v>
+      </c>
+    </row>
+    <row r="41">
+      <c r="A41" t="inlineStr">
+        <is>
+          <t>Ncpa Upcoming Events</t>
+        </is>
+      </c>
+      <c r="B41" t="inlineStr">
+        <is>
+          <t>NCPA Upcoming EventsThe Studio Theatre and Cube (NMACC)MIX OPEN MICSUNBURN - Upcoming EventsThe Daily Apple Laptop DJ WORKSHOPJamming Night - Valentines EditionVocal workshopSOI Spring 2026 SeasonThe DJ Blues 2 and 1 salsa elementary workshopSama'a: Festival of Sufi Music</t>
+        </is>
+      </c>
+      <c r="C41" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D41" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E41" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F41" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/ncpa-upcoming-events/ET00305288?webview=true</t>
+        </is>
+      </c>
+      <c r="G41" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H41" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I41" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:49</t>
+        </is>
+      </c>
+      <c r="J41" t="n">
+        <v>9113988627658034</v>
+      </c>
+    </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>Letters To Lata Didi By Shreya Ghoshal</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>Manoj Muntashir's Krishna - Radha Se Ranbhumi TakThe Grand Theatre, NMACCConcerts₹ 2500 onwardsManoj Muntashir's Krishna - Radha Se Ranbhumi TakLetters to Lata Didi by Shreya GhoshalJio World Garden, BKC: MumbaiConcerts₹ 2999 onwardsLetters to Lata Didi by Shreya GhoshalSama'a: Festival of Sufi Music - Day 3Tata Theatre: NCPAConcerts₹ 500 onwardsSama'a: Festival of Sufi Music - Day 3Doug Aitken: UNDER THE SUNArt House, Nita Mukesh Ambani Cultural CentreArt Exhibitions₹ 250 onwardsDoug Aitken: UNDER THE SUN</t>
+        </is>
+      </c>
+      <c r="C42" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D42" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E42" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/letters-to-lata-didi-by-shreya-ghoshal/ET00474204</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I42" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:48</t>
+        </is>
+      </c>
+      <c r="J42" t="n">
+        <v>8311854138617698</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>Doug Aitken Under The Sun</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>Manoj Muntashir's Krishna - Radha Se Ranbhumi TakThe Grand Theatre, NMACCConcerts₹ 2500 onwardsManoj Muntashir's Krishna - Radha Se Ranbhumi TakLetters to Lata Didi by Shreya GhoshalJio World Garden, BKC: MumbaiConcerts₹ 2999 onwardsLetters to Lata Didi by Shreya GhoshalSama'a: Festival of Sufi Music - Day 3Tata Theatre: NCPAConcerts₹ 500 onwardsSama'a: Festival of Sufi Music - Day 3Doug Aitken: UNDER THE SUNArt House, Nita Mukesh Ambani Cultural CentreArt Exhibitions₹ 250 onwardsDoug Aitken: UNDER THE SUN</t>
+        </is>
+      </c>
+      <c r="C43" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D43" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E43" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/doug-aitken-under-the-sun/ET00469533</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I43" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:48</t>
+        </is>
+      </c>
+      <c r="J43" t="n">
+        <v>9132104223511360</v>
+      </c>
+    </row>
+    <row r="44">
+      <c r="A44" t="inlineStr">
+        <is>
+          <t>Sama A Festival Of Sufi Music Day 3</t>
+        </is>
+      </c>
+      <c r="B44" t="inlineStr">
+        <is>
+          <t>Manoj Muntashir's Krishna - Radha Se Ranbhumi TakThe Grand Theatre, NMACCConcerts₹ 2500 onwardsManoj Muntashir's Krishna - Radha Se Ranbhumi TakLetters to Lata Didi by Shreya GhoshalJio World Garden, BKC: MumbaiConcerts₹ 2999 onwardsLetters to Lata Didi by Shreya GhoshalSama'a: Festival of Sufi Music - Day 3Tata Theatre: NCPAConcerts₹ 500 onwardsSama'a: Festival of Sufi Music - Day 3Doug Aitken: UNDER THE SUNArt House, Nita Mukesh Ambani Cultural CentreArt Exhibitions₹ 250 onwardsDoug Aitken: UNDER THE SUN</t>
+        </is>
+      </c>
+      <c r="C44" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D44" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E44" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F44" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/sama-a-festival-of-sufi-music-day-3/ET00480910</t>
+        </is>
+      </c>
+      <c r="G44" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H44" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I44" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:48</t>
+        </is>
+      </c>
+      <c r="J44" t="n">
+        <v>-462539575990560</v>
+      </c>
+    </row>
+    <row r="45">
+      <c r="A45" t="inlineStr">
+        <is>
+          <t>Sanam India Tour Mumbai</t>
+        </is>
+      </c>
+      <c r="B45" t="inlineStr">
+        <is>
+          <t>Main Shayar Toh Nahi- Manhar SethHotel Rang Sharda: MumbaiStand up Comedy₹ 499 onwardsMain Shayar Toh Nahi- Manhar SethSpoken Fest Mumbai 2026Jio World Garden, BKC: MumbaiSpoken Word₹ 999 onwardsSpoken Fest Mumbai 2026Sanam India Tour - MumbaiSouth Sky, Jio World Drive: MumbaiConcerts₹ 2999 onwardsSanam India Tour - MumbaiRough Jokes ft. Amit Tandon: KCCKhar Comedy Club: MumbaiStand up Comedy₹ 499Rough Jokes ft. Amit Tandon: KCC</t>
+        </is>
+      </c>
+      <c r="C45" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D45" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E45" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F45" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/sanam-india-tour-mumbai/ET00466356</t>
+        </is>
+      </c>
+      <c r="G45" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H45" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I45" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:47</t>
+        </is>
+      </c>
+      <c r="J45" t="n">
+        <v>-863857139495437</v>
+      </c>
+    </row>
+    <row r="46">
+      <c r="A46" t="inlineStr">
+        <is>
+          <t>Amit Tondon Live Kcc</t>
+        </is>
+      </c>
+      <c r="B46" t="inlineStr">
+        <is>
+          <t>Main Shayar Toh Nahi- Manhar SethHotel Rang Sharda: MumbaiStand up Comedy₹ 499 onwardsMain Shayar Toh Nahi- Manhar SethSpoken Fest Mumbai 2026Jio World Garden, BKC: MumbaiSpoken Word₹ 999 onwardsSpoken Fest Mumbai 2026Sanam India Tour - MumbaiSouth Sky, Jio World Drive: MumbaiConcerts₹ 2999 onwardsSanam India Tour - MumbaiRough Jokes ft. Amit Tandon: KCCKhar Comedy Club: MumbaiStand up Comedy₹ 499Rough Jokes ft. Amit Tandon: KCC</t>
+        </is>
+      </c>
+      <c r="C46" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D46" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E46" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F46" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/amit-tondon-live-kcc/ET00473247</t>
+        </is>
+      </c>
+      <c r="G46" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H46" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I46" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:47</t>
+        </is>
+      </c>
+      <c r="J46" t="n">
+        <v>7213896662123453</v>
+      </c>
+    </row>
+    <row r="47">
+      <c r="A47" t="inlineStr">
+        <is>
+          <t>Manoj Muntashir S Krishna Radha Se Ranbhumi Tak</t>
+        </is>
+      </c>
+      <c r="B47" t="inlineStr">
+        <is>
+          <t>Manoj Muntashir's Krishna - Radha Se Ranbhumi TakThe Grand Theatre, NMACCConcerts₹ 2500 onwardsManoj Muntashir's Krishna - Radha Se Ranbhumi TakLetters to Lata Didi by Shreya GhoshalJio World Garden, BKC: MumbaiConcerts₹ 2999 onwardsLetters to Lata Didi by Shreya GhoshalSama'a: Festival of Sufi Music - Day 3Tata Theatre: NCPAConcerts₹ 500 onwardsSama'a: Festival of Sufi Music - Day 3Doug Aitken: UNDER THE SUNArt House, Nita Mukesh Ambani Cultural CentreArt Exhibitions₹ 250 onwardsDoug Aitken: UNDER THE SUN</t>
+        </is>
+      </c>
+      <c r="C47" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D47" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E47" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F47" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/manoj-muntashir-s-krishna-radha-se-ranbhumi-tak/ET00482458</t>
+        </is>
+      </c>
+      <c r="G47" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H47" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I47" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:47</t>
+        </is>
+      </c>
+      <c r="J47" t="n">
+        <v>-300658533514382</v>
+      </c>
+    </row>
+    <row r="48">
+      <c r="A48" t="inlineStr">
+        <is>
+          <t>Spoken Fest Mumbai 2026</t>
+        </is>
+      </c>
+      <c r="B48" t="inlineStr">
+        <is>
+          <t>Main Shayar Toh Nahi- Manhar SethHotel Rang Sharda: MumbaiStand up Comedy₹ 499 onwardsMain Shayar Toh Nahi- Manhar SethSpoken Fest Mumbai 2026Jio World Garden, BKC: MumbaiSpoken Word₹ 999 onwardsSpoken Fest Mumbai 2026Sanam India Tour - MumbaiSouth Sky, Jio World Drive: MumbaiConcerts₹ 2999 onwardsSanam India Tour - MumbaiRough Jokes ft. Amit Tandon: KCCKhar Comedy Club: MumbaiStand up Comedy₹ 499Rough Jokes ft. Amit Tandon: KCC</t>
+        </is>
+      </c>
+      <c r="C48" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D48" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E48" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F48" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/spoken-fest-mumbai-2026/ET00458598</t>
+        </is>
+      </c>
+      <c r="G48" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H48" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I48" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:46</t>
+        </is>
+      </c>
+      <c r="J48" t="n">
+        <v>8178184370217172</v>
+      </c>
+    </row>
+    <row r="49">
+      <c r="A49" t="inlineStr">
+        <is>
+          <t>Main Shayar Toh Nahi Manhar Seth</t>
+        </is>
+      </c>
+      <c r="B49" t="inlineStr">
+        <is>
+          <t>Main Shayar Toh Nahi- Manhar SethHotel Rang Sharda: MumbaiStand up Comedy₹ 499 onwardsMain Shayar Toh Nahi- Manhar SethSpoken Fest Mumbai 2026Jio World Garden, BKC: MumbaiSpoken Word₹ 999 onwardsSpoken Fest Mumbai 2026Sanam India Tour - MumbaiSouth Sky, Jio World Drive: MumbaiConcerts₹ 2999 onwardsSanam India Tour - MumbaiRough Jokes ft. Amit Tandon: KCCKhar Comedy Club: MumbaiStand up Comedy₹ 499Rough Jokes ft. Amit Tandon: KCC</t>
+        </is>
+      </c>
+      <c r="C49" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D49" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E49" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F49" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/main-shayar-toh-nahi-manhar-seth/ET00469851</t>
+        </is>
+      </c>
+      <c r="G49" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H49" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I49" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:46</t>
+        </is>
+      </c>
+      <c r="J49" t="n">
+        <v>5909782130821593</v>
+      </c>
+    </row>
+    <row r="50">
+      <c r="A50" t="inlineStr">
+        <is>
+          <t>Toxic Abhishek Upmanyu Live</t>
+        </is>
+      </c>
+      <c r="B50" t="inlineStr">
+        <is>
+          <t>Halwa by Amit Tandon-NCPATata Theatre: NCPA.Stand up Comedy₹ 799 onwardsHalwa by Amit Tandon-NCPAJohn Mayer Solo - Live In Mumbai, 2026Mahalaxmi Race Course: MumbaiConcerts₹ 5000 onwardsJohn Mayer Solo - Live In Mumbai, 2026Mahindra Blues Festival 2026Mehboob Studios: Bandra(W)Concerts₹ 4000 onwardsMahindra Blues Festival 2026TOXIC - Abhishek Upmanyu LiveSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 799 onwardsTOXIC - Abhishek Upmanyu Live</t>
+        </is>
+      </c>
+      <c r="C50" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D50" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E50" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F50" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/toxic-abhishek-upmanyu-live/ET00409716</t>
+        </is>
+      </c>
+      <c r="G50" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H50" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I50" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:46</t>
+        </is>
+      </c>
+      <c r="J50" t="n">
+        <v>-875818091617151</v>
+      </c>
+    </row>
+    <row r="51">
+      <c r="A51" t="inlineStr">
+        <is>
+          <t>Mahindra Blues Festival 2026</t>
+        </is>
+      </c>
+      <c r="B51" t="inlineStr">
+        <is>
+          <t>Halwa by Amit Tandon-NCPATata Theatre: NCPA.Stand up Comedy₹ 799 onwardsHalwa by Amit Tandon-NCPAJohn Mayer Solo - Live In Mumbai, 2026Mahalaxmi Race Course: MumbaiConcerts₹ 5000 onwardsJohn Mayer Solo - Live In Mumbai, 2026Mahindra Blues Festival 2026Mehboob Studios: Bandra(W)Concerts₹ 4000 onwardsMahindra Blues Festival 2026TOXIC - Abhishek Upmanyu LiveSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 799 onwardsTOXIC - Abhishek Upmanyu Live</t>
+        </is>
+      </c>
+      <c r="C51" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D51" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E51" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F51" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/mahindra-blues-festival-2026/ET00468903</t>
+        </is>
+      </c>
+      <c r="G51" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H51" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I51" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:46</t>
+        </is>
+      </c>
+      <c r="J51" t="n">
+        <v>8047608815574611</v>
+      </c>
+    </row>
+    <row r="52">
+      <c r="A52" t="inlineStr">
+        <is>
+          <t>John Mayer Solo Live In Mumbai 2026</t>
+        </is>
+      </c>
+      <c r="B52" t="inlineStr">
+        <is>
+          <t>Halwa by Amit Tandon-NCPATata Theatre: NCPA.Stand up Comedy₹ 799 onwardsHalwa by Amit Tandon-NCPAJohn Mayer Solo - Live In Mumbai, 2026Mahalaxmi Race Course: MumbaiConcerts₹ 5000 onwardsJohn Mayer Solo - Live In Mumbai, 2026Mahindra Blues Festival 2026Mehboob Studios: Bandra(W)Concerts₹ 4000 onwardsMahindra Blues Festival 2026TOXIC - Abhishek Upmanyu LiveSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 799 onwardsTOXIC - Abhishek Upmanyu Live</t>
+        </is>
+      </c>
+      <c r="C52" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D52" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E52" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F52" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/john-mayer-solo-live-in-mumbai-2026/ET00464841</t>
+        </is>
+      </c>
+      <c r="G52" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H52" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I52" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:45</t>
+        </is>
+      </c>
+      <c r="J52" t="n">
+        <v>1830344615170119</v>
+      </c>
+    </row>
+    <row r="53">
+      <c r="A53" t="inlineStr">
+        <is>
+          <t>Halwa By Amit Tandon</t>
+        </is>
+      </c>
+      <c r="B53" t="inlineStr">
+        <is>
+          <t>Halwa by Amit Tandon-NCPATata Theatre: NCPA.Stand up Comedy₹ 799 onwardsHalwa by Amit Tandon-NCPAJohn Mayer Solo - Live In Mumbai, 2026Mahalaxmi Race Course: MumbaiConcerts₹ 5000 onwardsJohn Mayer Solo - Live In Mumbai, 2026Mahindra Blues Festival 2026Mehboob Studios: Bandra(W)Concerts₹ 4000 onwardsMahindra Blues Festival 2026TOXIC - Abhishek Upmanyu LiveSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 799 onwardsTOXIC - Abhishek Upmanyu Live</t>
+        </is>
+      </c>
+      <c r="C53" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D53" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E53" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F53" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/halwa-by-amit-tandon/ET00478732</t>
+        </is>
+      </c>
+      <c r="G53" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H53" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I53" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:45</t>
+        </is>
+      </c>
+      <c r="J53" t="n">
+        <v>-652733870842175</v>
+      </c>
+    </row>
+    <row r="54">
+      <c r="A54" t="inlineStr">
+        <is>
+          <t>Gaurav Gupta Live India Tour</t>
+        </is>
+      </c>
+      <c r="B54" t="inlineStr">
+        <is>
+          <t>Anuv Jain - Dastakhat India Tour (Mumbai)DOME, SVP Stadium: MumbaiConcerts₹ 2500 onwardsAnuv Jain - Dastakhat India Tour (Mumbai)CALVIN HARRIS - Live in MumbaiInfinity Bay: MumbaiConcerts₹ 3000 onwardsCALVIN HARRIS - Live in MumbaiBhajan Clubbing - The New Wave of DevotionRangasharda Auditorium: MumbaiConcerts₹ 299 onwardsBhajan Clubbing - The New Wave of DevotionGaurav Gupta Live - India TourFine Arts Society (Sivaswamy Auditorium): ChemburStand up Comedy₹ 799 onwardsGaurav Gupta Live - India Tour</t>
+        </is>
+      </c>
+      <c r="C54" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D54" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E54" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F54" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/gaurav-gupta-live-india-tour/ET00358468</t>
+        </is>
+      </c>
+      <c r="G54" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H54" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I54" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:45</t>
+        </is>
+      </c>
+      <c r="J54" t="n">
+        <v>8649810493320537</v>
+      </c>
+    </row>
+    <row r="55">
+      <c r="A55" t="inlineStr">
+        <is>
+          <t>Bhajan Clubbing The New Wave Of Devotion</t>
+        </is>
+      </c>
+      <c r="B55" t="inlineStr">
+        <is>
+          <t>Anuv Jain - Dastakhat India Tour (Mumbai)DOME, SVP Stadium: MumbaiConcerts₹ 2500 onwardsAnuv Jain - Dastakhat India Tour (Mumbai)CALVIN HARRIS - Live in MumbaiInfinity Bay: MumbaiConcerts₹ 3000 onwardsCALVIN HARRIS - Live in MumbaiBhajan Clubbing - The New Wave of DevotionRangasharda Auditorium: MumbaiConcerts₹ 299 onwardsBhajan Clubbing - The New Wave of DevotionGaurav Gupta Live - India TourFine Arts Society (Sivaswamy Auditorium): ChemburStand up Comedy₹ 799 onwardsGaurav Gupta Live - India Tour</t>
+        </is>
+      </c>
+      <c r="C55" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D55" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E55" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F55" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/bhajan-clubbing-the-new-wave-of-devotion/ET00481773</t>
+        </is>
+      </c>
+      <c r="G55" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H55" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I55" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:44</t>
+        </is>
+      </c>
+      <c r="J55" t="n">
+        <v>3666724037004160</v>
+      </c>
+    </row>
+    <row r="56">
+      <c r="A56" t="inlineStr">
+        <is>
+          <t>Calvin Harris Live In Mumbai</t>
+        </is>
+      </c>
+      <c r="B56" t="inlineStr">
+        <is>
+          <t>Anuv Jain - Dastakhat India Tour (Mumbai)DOME, SVP Stadium: MumbaiConcerts₹ 2500 onwardsAnuv Jain - Dastakhat India Tour (Mumbai)CALVIN HARRIS - Live in MumbaiInfinity Bay: MumbaiConcerts₹ 3000 onwardsCALVIN HARRIS - Live in MumbaiBhajan Clubbing - The New Wave of DevotionRangasharda Auditorium: MumbaiConcerts₹ 299 onwardsBhajan Clubbing - The New Wave of DevotionGaurav Gupta Live - India TourFine Arts Society (Sivaswamy Auditorium): ChemburStand up Comedy₹ 799 onwardsGaurav Gupta Live - India Tour</t>
+        </is>
+      </c>
+      <c r="C56" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D56" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E56" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F56" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/calvin-harris-live-in-mumbai/ET00462236</t>
+        </is>
+      </c>
+      <c r="G56" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H56" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I56" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:44</t>
+        </is>
+      </c>
+      <c r="J56" t="n">
+        <v>6301505570597666</v>
+      </c>
+    </row>
+    <row r="57">
+      <c r="A57" t="inlineStr">
+        <is>
+          <t>Anuv Jain Dastakhat India Tour Mumbai</t>
+        </is>
+      </c>
+      <c r="B57" t="inlineStr">
+        <is>
+          <t>Anuv Jain - Dastakhat India Tour (Mumbai)DOME, SVP Stadium: MumbaiConcerts₹ 2500 onwardsAnuv Jain - Dastakhat India Tour (Mumbai)CALVIN HARRIS - Live in MumbaiInfinity Bay: MumbaiConcerts₹ 3000 onwardsCALVIN HARRIS - Live in MumbaiBhajan Clubbing - The New Wave of DevotionRangasharda Auditorium: MumbaiConcerts₹ 299 onwardsBhajan Clubbing - The New Wave of DevotionGaurav Gupta Live - India TourFine Arts Society (Sivaswamy Auditorium): ChemburStand up Comedy₹ 799 onwardsGaurav Gupta Live - India Tour</t>
+        </is>
+      </c>
+      <c r="C57" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D57" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E57" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F57" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/anuv-jain-dastakhat-india-tour-mumbai/ET00470487</t>
+        </is>
+      </c>
+      <c r="G57" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H57" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I57" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:44</t>
+        </is>
+      </c>
+      <c r="J57" t="n">
+        <v>6193409027485856</v>
+      </c>
+    </row>
+    <row r="58">
+      <c r="A58" t="inlineStr">
+        <is>
+          <t>Keinemusik Live In Mumbai</t>
+        </is>
+      </c>
+      <c r="B58" t="inlineStr">
+        <is>
+          <t>Daily Ka Kaam Hai By Aakash Gupta - MumbaiSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 599 onwardsDaily Ka Kaam Hai By Aakash Gupta - MumbaiLove, Death &amp; Ketchup by Varun GroverBal Gandharva Rang Mandir: MumbaiStand up Comedy₹ 799 onwardsLove, Death &amp; Ketchup by Varun GroverKeinemusik - Live in MumbaiMahalaxmi Race Course: MumbaiConcerts₹ 3500 onwardsKeinemusik - Live in MumbaiSama'a: Festival of Sufi Music - Day 2Tata Theatre: NCPAConcerts₹ 300 onwardsSama'a: Festival of Sufi Music - Day 2</t>
+        </is>
+      </c>
+      <c r="C58" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D58" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E58" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F58" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/keinemusik-live-in-mumbai/ET00467697</t>
+        </is>
+      </c>
+      <c r="G58" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H58" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I58" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:43</t>
+        </is>
+      </c>
+      <c r="J58" t="n">
+        <v>-119528849040579</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>Love Death Ketchup By Varun Grover</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>Daily Ka Kaam Hai By Aakash Gupta - MumbaiSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 599 onwardsDaily Ka Kaam Hai By Aakash Gupta - MumbaiLove, Death &amp; Ketchup by Varun GroverBal Gandharva Rang Mandir: MumbaiStand up Comedy₹ 799 onwardsLove, Death &amp; Ketchup by Varun GroverKeinemusik - Live in MumbaiMahalaxmi Race Course: MumbaiConcerts₹ 3500 onwardsKeinemusik - Live in MumbaiSama'a: Festival of Sufi Music - Day 2Tata Theatre: NCPAConcerts₹ 300 onwardsSama'a: Festival of Sufi Music - Day 2</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D59" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E59" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F59" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/love-death-ketchup-by-varun-grover/ET00466188</t>
+        </is>
+      </c>
+      <c r="G59" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H59" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I59" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:43</t>
+        </is>
+      </c>
+      <c r="J59" t="n">
+        <v>-599795242289484</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>Sama A Festival Of Sufi Music Day 2</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>Daily Ka Kaam Hai By Aakash Gupta - MumbaiSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 599 onwardsDaily Ka Kaam Hai By Aakash Gupta - MumbaiLove, Death &amp; Ketchup by Varun GroverBal Gandharva Rang Mandir: MumbaiStand up Comedy₹ 799 onwardsLove, Death &amp; Ketchup by Varun GroverKeinemusik - Live in MumbaiMahalaxmi Race Course: MumbaiConcerts₹ 3500 onwardsKeinemusik - Live in MumbaiSama'a: Festival of Sufi Music - Day 2Tata Theatre: NCPAConcerts₹ 300 onwardsSama'a: Festival of Sufi Music - Day 2</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D60" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E60" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F60" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/sama-a-festival-of-sufi-music-day-2/ET00480908</t>
+        </is>
+      </c>
+      <c r="G60" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H60" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I60" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:43</t>
+        </is>
+      </c>
+      <c r="J60" t="n">
+        <v>-321794354107730</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>Daily Ka Kaam Hai By Aakash Gupta Mumbai</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>Daily Ka Kaam Hai By Aakash Gupta - MumbaiSophia Bhabha Auditorium: MumbaiStand up Comedy₹ 599 onwardsDaily Ka Kaam Hai By Aakash Gupta - MumbaiLove, Death &amp; Ketchup by Varun GroverBal Gandharva Rang Mandir: MumbaiStand up Comedy₹ 799 onwardsLove, Death &amp; Ketchup by Varun GroverKeinemusik - Live in MumbaiMahalaxmi Race Course: MumbaiConcerts₹ 3500 onwardsKeinemusik - Live in MumbaiSama'a: Festival of Sufi Music - Day 2Tata Theatre: NCPAConcerts₹ 300 onwardsSama'a: Festival of Sufi Music - Day 2</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>Various Venues</t>
+        </is>
+      </c>
+      <c r="D61" t="inlineStr">
+        <is>
+          <t>Mumbai</t>
+        </is>
+      </c>
+      <c r="E61" t="inlineStr">
+        <is>
+          <t>General</t>
+        </is>
+      </c>
+      <c r="F61" t="inlineStr">
+        <is>
+          <t>https://in.bookmyshow.com/events/daily-ka-kaam-hai-by-aakash-gupta-mumbai/ET00429299</t>
+        </is>
+      </c>
+      <c r="G61" t="inlineStr">
+        <is>
+          <t>BookMyShow</t>
+        </is>
+      </c>
+      <c r="H61" t="inlineStr">
+        <is>
+          <t>Active</t>
+        </is>
+      </c>
+      <c r="I61" t="inlineStr">
+        <is>
+          <t>2026-02-03 18:14:43</t>
+        </is>
+      </c>
+      <c r="J61" t="n">
+        <v>8801684389609160</v>
       </c>
     </row>
   </sheetData>

</xml_diff>